<commit_message>
add Academic Number column
</commit_message>
<xml_diff>
--- a/csv/registered_ids.xlsx
+++ b/csv/registered_ids.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\Desktop\RFID Attendance\csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A9FE0A5-B123-47DF-804B-F06B4B200FC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8D4D4FF-EB19-43D1-85A4-166B57D0696A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5CF634DC-0562-40CA-83C8-C14B325D483F}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>ID</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t>6C 0E 84 B9</t>
+  </si>
+  <si>
+    <t>Academic Number</t>
   </si>
 </sst>
 </file>
@@ -413,18 +416,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16F56AB6-613B-4EA4-A278-9C2ECBA1C0D8}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -434,8 +438,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -445,8 +452,11 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
+      <c r="D2">
+        <v>12345</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -455,6 +465,9 @@
       </c>
       <c r="C3" t="s">
         <v>6</v>
+      </c>
+      <c r="D3">
+        <v>77225</v>
       </c>
     </row>
   </sheetData>

</xml_diff>